<commit_message>
Case beskrivelser næsten færdig + lidt rettelser
</commit_message>
<xml_diff>
--- a/Simulerings resultater.xlsx
+++ b/Simulerings resultater.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lauri\Documents\Energy System Stability project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E33BB866-CF7F-4CBD-A860-CFFF892AE59A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F8E212E-0E71-483F-8E79-C2D57C9E1C0F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -91,13 +91,13 @@
 Disconnection of town 2 at trafo</t>
   </si>
   <si>
-    <t>Big disturbance w. decentral batterieris, 60kV transmissions cable out for maintanence, loss of Windfarm (2MW and pf 0,95), full load (1,5MW and pf 0,95)</t>
+    <t>Batterypark</t>
   </si>
   <si>
-    <t>Big disturbance w. central batteryprak, 60kV transmissions cable out for maintanence, loss of Windfarm (2MW and pf 0,95), full load (1,5MW and pf 0,95)</t>
+    <t>Big disturbance w. decentral batterieries, 60kV transmissions cable out for maintanence, loss of Windfarm (2MW and pf 0,95), full load (1,5MW and pf 0,95)</t>
   </si>
   <si>
-    <t>Batterypark</t>
+    <t>Big disturbance w. central batterypark, 60kV transmissions cable out for maintanence, loss of Windfarm (2MW and pf 0,95), full load (1,5MW and pf 0,95)</t>
   </si>
 </sst>
 </file>
@@ -286,17 +286,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -304,8 +295,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -589,8 +589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="V46" sqref="V46"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M21" sqref="M21:N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -611,32 +611,32 @@
   <sheetData>
     <row r="1" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="18">
-        <v>1</v>
-      </c>
-      <c r="D2" s="19"/>
-      <c r="E2" s="18">
+      <c r="B2" s="20"/>
+      <c r="C2" s="21">
+        <v>1</v>
+      </c>
+      <c r="D2" s="22"/>
+      <c r="E2" s="21">
         <v>2</v>
       </c>
-      <c r="F2" s="19"/>
-      <c r="G2" s="18">
+      <c r="F2" s="22"/>
+      <c r="G2" s="21">
         <v>3</v>
       </c>
-      <c r="H2" s="19"/>
-      <c r="I2" s="18">
+      <c r="H2" s="22"/>
+      <c r="I2" s="21">
         <v>4</v>
       </c>
-      <c r="J2" s="19"/>
-      <c r="K2" s="24"/>
-      <c r="L2" s="24"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
     </row>
     <row r="3" spans="1:12" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="22"/>
-      <c r="B3" s="23"/>
+      <c r="A3" s="19"/>
+      <c r="B3" s="20"/>
       <c r="C3" s="7" t="s">
         <v>13</v>
       </c>
@@ -665,7 +665,7 @@
       <c r="L3" s="1"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -697,7 +697,7 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="20"/>
+      <c r="A5" s="18"/>
       <c r="B5" s="5" t="s">
         <v>9</v>
       </c>
@@ -727,7 +727,7 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="20"/>
+      <c r="A6" s="18"/>
       <c r="B6" s="5" t="s">
         <v>10</v>
       </c>
@@ -1074,50 +1074,50 @@
     </row>
     <row r="20" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="21" spans="1:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" s="23"/>
-      <c r="C21" s="18">
-        <v>1</v>
-      </c>
-      <c r="D21" s="19"/>
-      <c r="E21" s="18">
+      <c r="A21" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="20"/>
+      <c r="C21" s="21">
+        <v>1</v>
+      </c>
+      <c r="D21" s="22"/>
+      <c r="E21" s="21">
         <v>2</v>
       </c>
-      <c r="F21" s="19"/>
-      <c r="G21" s="18">
+      <c r="F21" s="22"/>
+      <c r="G21" s="21">
         <v>3</v>
       </c>
-      <c r="H21" s="19"/>
-      <c r="I21" s="18">
+      <c r="H21" s="22"/>
+      <c r="I21" s="21">
         <v>4</v>
       </c>
-      <c r="J21" s="19"/>
-      <c r="M21" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="N21" s="23"/>
-      <c r="O21" s="18">
-        <v>1</v>
-      </c>
-      <c r="P21" s="19"/>
-      <c r="Q21" s="18">
+      <c r="J21" s="22"/>
+      <c r="M21" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="N21" s="20"/>
+      <c r="O21" s="21">
+        <v>1</v>
+      </c>
+      <c r="P21" s="22"/>
+      <c r="Q21" s="21">
         <v>2</v>
       </c>
-      <c r="R21" s="19"/>
-      <c r="S21" s="18">
+      <c r="R21" s="22"/>
+      <c r="S21" s="21">
         <v>3</v>
       </c>
-      <c r="T21" s="19"/>
-      <c r="U21" s="18">
+      <c r="T21" s="22"/>
+      <c r="U21" s="21">
         <v>4</v>
       </c>
-      <c r="V21" s="19"/>
+      <c r="V21" s="22"/>
     </row>
     <row r="22" spans="1:22" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A22" s="22"/>
-      <c r="B22" s="23"/>
+      <c r="A22" s="19"/>
+      <c r="B22" s="20"/>
       <c r="C22" s="15" t="s">
         <v>13</v>
       </c>
@@ -1142,8 +1142,8 @@
       <c r="J22" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="M22" s="22"/>
-      <c r="N22" s="23"/>
+      <c r="M22" s="19"/>
+      <c r="N22" s="20"/>
       <c r="O22" s="15" t="s">
         <v>13</v>
       </c>
@@ -1170,7 +1170,7 @@
       </c>
     </row>
     <row r="23" spans="1:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="20" t="s">
+      <c r="A23" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B23" s="5" t="s">
@@ -1200,7 +1200,7 @@
       <c r="J23" s="10">
         <v>0.13700000000000001</v>
       </c>
-      <c r="M23" s="20" t="s">
+      <c r="M23" s="18" t="s">
         <v>0</v>
       </c>
       <c r="N23" s="5" t="s">
@@ -1232,7 +1232,7 @@
       </c>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A24" s="20"/>
+      <c r="A24" s="18"/>
       <c r="B24" s="5" t="s">
         <v>9</v>
       </c>
@@ -1260,7 +1260,7 @@
       <c r="J24" s="10">
         <v>-3.536</v>
       </c>
-      <c r="M24" s="20"/>
+      <c r="M24" s="18"/>
       <c r="N24" s="5" t="s">
         <v>9</v>
       </c>
@@ -1290,7 +1290,7 @@
       </c>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A25" s="20"/>
+      <c r="A25" s="18"/>
       <c r="B25" s="5" t="s">
         <v>10</v>
       </c>
@@ -1318,7 +1318,7 @@
       <c r="J25" s="10">
         <v>0.98</v>
       </c>
-      <c r="M25" s="20"/>
+      <c r="M25" s="18"/>
       <c r="N25" s="5" t="s">
         <v>10</v>
       </c>
@@ -2320,7 +2320,7 @@
       </c>
     </row>
     <row r="42" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A42" s="21"/>
+      <c r="A42" s="24"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
@@ -2331,7 +2331,7 @@
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
       <c r="M42" s="17" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="N42" s="6" t="s">
         <v>8</v>
@@ -2362,7 +2362,7 @@
       </c>
     </row>
     <row r="43" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="21"/>
+      <c r="A43" s="24"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
@@ -2402,7 +2402,7 @@
       </c>
     </row>
     <row r="44" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A44" s="21"/>
+      <c r="A44" s="24"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
@@ -2414,7 +2414,7 @@
       <c r="J44" s="2"/>
     </row>
     <row r="45" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="21"/>
+      <c r="A45" s="24"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
@@ -2426,30 +2426,30 @@
       <c r="J45" s="2"/>
     </row>
     <row r="46" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A46" s="22" t="s">
+      <c r="A46" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="B46" s="23"/>
-      <c r="C46" s="18">
-        <v>1</v>
-      </c>
-      <c r="D46" s="19"/>
-      <c r="E46" s="18">
+      <c r="B46" s="20"/>
+      <c r="C46" s="21">
+        <v>1</v>
+      </c>
+      <c r="D46" s="22"/>
+      <c r="E46" s="21">
         <v>2</v>
       </c>
-      <c r="F46" s="19"/>
-      <c r="G46" s="18">
+      <c r="F46" s="22"/>
+      <c r="G46" s="21">
         <v>3</v>
       </c>
-      <c r="H46" s="19"/>
-      <c r="I46" s="18">
+      <c r="H46" s="22"/>
+      <c r="I46" s="21">
         <v>4</v>
       </c>
-      <c r="J46" s="19"/>
+      <c r="J46" s="22"/>
     </row>
     <row r="47" spans="1:22" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A47" s="22"/>
-      <c r="B47" s="23"/>
+      <c r="A47" s="19"/>
+      <c r="B47" s="20"/>
       <c r="C47" s="15" t="s">
         <v>13</v>
       </c>
@@ -2476,7 +2476,7 @@
       </c>
     </row>
     <row r="48" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A48" s="20" t="s">
+      <c r="A48" s="18" t="s">
         <v>0</v>
       </c>
       <c r="B48" s="5" t="s">
@@ -2500,7 +2500,7 @@
       <c r="J48" s="10"/>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A49" s="20"/>
+      <c r="A49" s="18"/>
       <c r="B49" s="5" t="s">
         <v>9</v>
       </c>
@@ -2522,7 +2522,7 @@
       <c r="J49" s="10"/>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A50" s="20"/>
+      <c r="A50" s="18"/>
       <c r="B50" s="5" t="s">
         <v>10</v>
       </c>
@@ -2919,27 +2919,17 @@
     </row>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="M40:M41"/>
-    <mergeCell ref="M42:M43"/>
-    <mergeCell ref="M23:M25"/>
-    <mergeCell ref="M32:M33"/>
-    <mergeCell ref="M34:M35"/>
-    <mergeCell ref="M36:M37"/>
-    <mergeCell ref="M38:M39"/>
-    <mergeCell ref="M21:N22"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="Q21:R21"/>
-    <mergeCell ref="S21:T21"/>
-    <mergeCell ref="U21:V21"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="A59:A60"/>
+    <mergeCell ref="A61:A62"/>
+    <mergeCell ref="A63:A64"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="G46:H46"/>
+    <mergeCell ref="I46:J46"/>
+    <mergeCell ref="A48:A50"/>
+    <mergeCell ref="A57:A58"/>
+    <mergeCell ref="A46:B47"/>
     <mergeCell ref="A40:A41"/>
     <mergeCell ref="A42:A43"/>
     <mergeCell ref="A44:A45"/>
@@ -2953,17 +2943,27 @@
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="A15:A16"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="G46:H46"/>
-    <mergeCell ref="I46:J46"/>
-    <mergeCell ref="A48:A50"/>
-    <mergeCell ref="A57:A58"/>
-    <mergeCell ref="A46:B47"/>
-    <mergeCell ref="A59:A60"/>
-    <mergeCell ref="A61:A62"/>
-    <mergeCell ref="A63:A64"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="M21:N22"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="Q21:R21"/>
+    <mergeCell ref="S21:T21"/>
+    <mergeCell ref="U21:V21"/>
+    <mergeCell ref="M40:M41"/>
+    <mergeCell ref="M42:M43"/>
+    <mergeCell ref="M23:M25"/>
+    <mergeCell ref="M32:M33"/>
+    <mergeCell ref="M34:M35"/>
+    <mergeCell ref="M36:M37"/>
+    <mergeCell ref="M38:M39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>